<commit_message>
Sincronización limpia de datos de finanzas
</commit_message>
<xml_diff>
--- a/2025 10 13 - SGA MOD - V31 - send 1.xlsx
+++ b/2025 10 13 - SGA MOD - V31 - send 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tilprafi\Desktop\Practica DP fin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C38D258-0EE0-4439-9BE7-E12F7796A5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A2CCB-E360-4B10-81A1-4B7FC438681A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="794" activeTab="2" xr2:uid="{1F6569A4-60A1-425C-9C9C-CCD538F6FF17}"/>
   </bookViews>
@@ -63005,7 +63005,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>

</xml_diff>